<commit_message>
Update of Horizontal yagi work
</commit_message>
<xml_diff>
--- a/antennas/MBSpanel_2/data/R descriptive stats body.xlsx
+++ b/antennas/MBSpanel_2/data/R descriptive stats body.xlsx
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>689510</v>
+        <v>689462</v>
       </c>
       <c r="C2" t="n">
         <v>1.84</v>
@@ -513,13 +513,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>689510</v>
+        <v>689462</v>
       </c>
       <c r="C3" t="n">
-        <v>3.36</v>
+        <v>2.32</v>
       </c>
       <c r="D3" t="n">
-        <v>280.69</v>
+        <v>0.29</v>
       </c>
       <c r="E3" t="n">
         <v>0.25</v>
@@ -534,7 +534,7 @@
         <v>2.41</v>
       </c>
       <c r="I3" t="n">
-        <v>116966.09</v>
+        <v>51.36</v>
       </c>
     </row>
     <row r="4">
@@ -544,13 +544,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>689510</v>
+        <v>689462</v>
       </c>
       <c r="C4" t="n">
-        <v>4.02</v>
+        <v>2.49</v>
       </c>
       <c r="D4" t="n">
-        <v>550.4400000000001</v>
+        <v>0.54</v>
       </c>
       <c r="E4" t="n">
         <v>0.2</v>
@@ -565,7 +565,7 @@
         <v>2.71</v>
       </c>
       <c r="I4" t="n">
-        <v>287983.05</v>
+        <v>123.82</v>
       </c>
     </row>
     <row r="5">
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>689510</v>
+        <v>689462</v>
       </c>
       <c r="C5" t="n">
-        <v>4.94</v>
+        <v>2.72</v>
       </c>
       <c r="D5" t="n">
-        <v>897.46</v>
+        <v>0.97</v>
       </c>
       <c r="E5" t="n">
         <v>0.16</v>
@@ -596,7 +596,7 @@
         <v>3.17</v>
       </c>
       <c r="I5" t="n">
-        <v>479966.6</v>
+        <v>205.83</v>
       </c>
     </row>
     <row r="6">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>689510</v>
+        <v>689462</v>
       </c>
       <c r="C6" t="n">
-        <v>4.01</v>
+        <v>2.48</v>
       </c>
       <c r="D6" t="n">
-        <v>550.4400000000001</v>
+        <v>0.52</v>
       </c>
       <c r="E6" t="n">
         <v>0.15</v>
@@ -627,7 +627,7 @@
         <v>2.7</v>
       </c>
       <c r="I6" t="n">
-        <v>287983.05</v>
+        <v>92.42</v>
       </c>
     </row>
     <row r="7">
@@ -637,13 +637,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>689510</v>
+        <v>689462</v>
       </c>
       <c r="C7" t="n">
-        <v>2.15</v>
+        <v>1.97</v>
       </c>
       <c r="D7" t="n">
-        <v>136.98</v>
+        <v>0.58</v>
       </c>
       <c r="E7" t="n">
         <v>0.09</v>
@@ -658,7 +658,7 @@
         <v>2.46</v>
       </c>
       <c r="I7" t="n">
-        <v>113612.79</v>
+        <v>27.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>